<commit_message>
Ideal Data Collection Progress Rate and Fixes in data
</commit_message>
<xml_diff>
--- a/03_analysis_input/adults_HiTOP_subscales.xlsx
+++ b/03_analysis_input/adults_HiTOP_subscales.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AC347"/>
+  <dimension ref="A1:AC346"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -12521,64 +12521,64 @@
     </row>
     <row r="137">
       <c r="A137">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="B137">
-        <v>0.15</v>
+        <v>0.35</v>
       </c>
       <c r="C137">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D137">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E137">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F137">
         <v>5</v>
       </c>
       <c r="G137">
+        <v>7</v>
+      </c>
+      <c r="H137">
         <v>11</v>
       </c>
-      <c r="H137">
-        <v>25</v>
-      </c>
       <c r="I137">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="J137">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="K137">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="L137">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="M137">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="N137">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="O137">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="P137">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="Q137">
         <v>6</v>
       </c>
       <c r="R137">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="S137">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="T137">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="U137">
         <v>7</v>
@@ -12610,64 +12610,64 @@
     </row>
     <row r="138">
       <c r="A138">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="B138">
-        <v>0.35</v>
+        <v>0.15</v>
       </c>
       <c r="C138">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="D138">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E138">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F138">
         <v>5</v>
       </c>
       <c r="G138">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="H138">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="I138">
+        <v>25</v>
+      </c>
+      <c r="J138">
+        <v>6</v>
+      </c>
+      <c r="K138">
         <v>15</v>
       </c>
-      <c r="J138">
-        <v>5</v>
-      </c>
-      <c r="K138">
-        <v>10</v>
-      </c>
       <c r="L138">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="M138">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="N138">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="O138">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="P138">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="Q138">
         <v>6</v>
       </c>
       <c r="R138">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="S138">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="T138">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="U138">
         <v>7</v>
@@ -12788,19 +12788,19 @@
     </row>
     <row r="140">
       <c r="A140">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="B140">
-        <v>0.05</v>
+        <v>0.25</v>
       </c>
       <c r="C140">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D140">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E140">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F140">
         <v>5</v>
@@ -12812,55 +12812,55 @@
         <v>17</v>
       </c>
       <c r="I140">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="J140">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="K140">
+        <v>14</v>
+      </c>
+      <c r="L140">
+        <v>11</v>
+      </c>
+      <c r="M140">
         <v>10</v>
       </c>
-      <c r="L140">
-        <v>8</v>
-      </c>
-      <c r="M140">
-        <v>5</v>
-      </c>
       <c r="N140">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="O140">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="P140">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="Q140">
         <v>6</v>
       </c>
       <c r="R140">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="S140">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="T140">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="U140">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="V140">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W140">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X140">
         <v>0</v>
       </c>
       <c r="Y140">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z140">
         <v>0</v>
@@ -12872,24 +12872,24 @@
         <v>0</v>
       </c>
       <c r="AC140">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="141">
       <c r="A141">
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="B141">
-        <v>0.25</v>
+        <v>0.05</v>
       </c>
       <c r="C141">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D141">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E141">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F141">
         <v>5</v>
@@ -12901,55 +12901,55 @@
         <v>17</v>
       </c>
       <c r="I141">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J141">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="K141">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="L141">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="M141">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="N141">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="O141">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="P141">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="Q141">
         <v>6</v>
       </c>
       <c r="R141">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="S141">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="T141">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="U141">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="V141">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W141">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X141">
         <v>0</v>
       </c>
       <c r="Y141">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z141">
         <v>0</v>
@@ -12961,7 +12961,7 @@
         <v>0</v>
       </c>
       <c r="AC141">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="142">
@@ -13678,67 +13678,67 @@
     </row>
     <row r="150">
       <c r="A150">
+        <v>0.05</v>
+      </c>
+      <c r="B150">
         <v>0.15</v>
       </c>
-      <c r="B150">
-        <v>0.35</v>
-      </c>
       <c r="C150">
         <v>4</v>
       </c>
       <c r="D150">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E150">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F150">
         <v>5</v>
       </c>
       <c r="G150">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="H150">
         <v>19</v>
       </c>
       <c r="I150">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="J150">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="K150">
         <v>8</v>
       </c>
       <c r="L150">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="M150">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="N150">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="O150">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="P150">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="Q150">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="R150">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="S150">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="T150">
         <v>23</v>
       </c>
       <c r="U150">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="V150">
         <v>1</v>
@@ -13762,72 +13762,72 @@
         <v>0</v>
       </c>
       <c r="AC150">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="151">
       <c r="A151">
-        <v>0.05</v>
+        <v>0.15</v>
       </c>
       <c r="B151">
-        <v>0.15</v>
+        <v>0.35</v>
       </c>
       <c r="C151">
         <v>4</v>
       </c>
       <c r="D151">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E151">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F151">
         <v>5</v>
       </c>
       <c r="G151">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="H151">
         <v>19</v>
       </c>
       <c r="I151">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="J151">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="K151">
         <v>8</v>
       </c>
       <c r="L151">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="M151">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="N151">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="O151">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="P151">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="Q151">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="R151">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="S151">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="T151">
         <v>23</v>
       </c>
       <c r="U151">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="V151">
         <v>1</v>
@@ -13851,7 +13851,7 @@
         <v>0</v>
       </c>
       <c r="AC151">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="152">
@@ -28419,13 +28419,13 @@
     </row>
     <row r="316">
       <c r="A316">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="B316">
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
       <c r="C316">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D316">
         <v>3</v>
@@ -28437,10 +28437,10 @@
         <v>5</v>
       </c>
       <c r="G316">
+        <v>7</v>
+      </c>
+      <c r="H316">
         <v>13</v>
-      </c>
-      <c r="H316">
-        <v>12</v>
       </c>
       <c r="I316">
         <v>25</v>
@@ -28449,43 +28449,43 @@
         <v>4</v>
       </c>
       <c r="K316">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="L316">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="M316">
         <v>5</v>
       </c>
       <c r="N316">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="O316">
         <v>8</v>
       </c>
       <c r="P316">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="Q316">
         <v>6</v>
       </c>
       <c r="R316">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="S316">
         <v>4</v>
       </c>
       <c r="T316">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="U316">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="V316">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="W316">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X316">
         <v>0</v>
@@ -28500,21 +28500,21 @@
         <v>0</v>
       </c>
       <c r="AB316">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC316">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="317">
       <c r="A317">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="B317">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="C317">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D317">
         <v>3</v>
@@ -28526,13 +28526,13 @@
         <v>5</v>
       </c>
       <c r="G317">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="H317">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="I317">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J317">
         <v>4</v>
@@ -28541,31 +28541,31 @@
         <v>6</v>
       </c>
       <c r="L317">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="M317">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="N317">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="O317">
         <v>8</v>
       </c>
       <c r="P317">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="Q317">
         <v>6</v>
       </c>
       <c r="R317">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="S317">
         <v>4</v>
       </c>
       <c r="T317">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="U317">
         <v>3</v>
@@ -28592,15 +28592,15 @@
         <v>0</v>
       </c>
       <c r="AC317">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="318">
       <c r="A318">
-        <v>0.05</v>
+        <v>0</v>
       </c>
       <c r="B318">
-        <v>0.05</v>
+        <v>0</v>
       </c>
       <c r="C318">
         <v>3</v>
@@ -28615,13 +28615,13 @@
         <v>5</v>
       </c>
       <c r="G318">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="H318">
         <v>11</v>
       </c>
       <c r="I318">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="J318">
         <v>4</v>
@@ -28630,19 +28630,19 @@
         <v>6</v>
       </c>
       <c r="L318">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="M318">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="N318">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="O318">
         <v>8</v>
       </c>
       <c r="P318">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="Q318">
         <v>6</v>
@@ -28654,13 +28654,13 @@
         <v>4</v>
       </c>
       <c r="T318">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="U318">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="V318">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W318">
         <v>0</v>
@@ -28698,16 +28698,16 @@
         <v>3</v>
       </c>
       <c r="E319">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F319">
         <v>5</v>
       </c>
       <c r="G319">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H319">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="I319">
         <v>25</v>
@@ -28716,16 +28716,16 @@
         <v>4</v>
       </c>
       <c r="K319">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="L319">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="M319">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="N319">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="O319">
         <v>8</v>
@@ -28743,10 +28743,10 @@
         <v>4</v>
       </c>
       <c r="T319">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="U319">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="V319">
         <v>1</v>
@@ -28770,36 +28770,36 @@
         <v>0</v>
       </c>
       <c r="AC319">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="320">
       <c r="A320">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="B320">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="C320">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D320">
         <v>3</v>
       </c>
       <c r="E320">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F320">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G320">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H320">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="I320">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="J320">
         <v>4</v>
@@ -28808,19 +28808,19 @@
         <v>7</v>
       </c>
       <c r="L320">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="M320">
         <v>7</v>
       </c>
       <c r="N320">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="O320">
         <v>8</v>
       </c>
       <c r="P320">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="Q320">
         <v>6</v>
@@ -28829,13 +28829,13 @@
         <v>4</v>
       </c>
       <c r="S320">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="T320">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="U320">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="V320">
         <v>1</v>
@@ -28859,72 +28859,72 @@
         <v>0</v>
       </c>
       <c r="AC320">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="321">
       <c r="A321">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="B321">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="C321">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D321">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="E321">
         <v>3</v>
       </c>
       <c r="F321">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G321">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="H321">
-        <v>12</v>
+        <v>41</v>
       </c>
       <c r="I321">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="J321">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="K321">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="L321">
-        <v>6</v>
+        <v>27</v>
       </c>
       <c r="M321">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="N321">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="O321">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="P321">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="Q321">
         <v>6</v>
       </c>
       <c r="R321">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="S321">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="T321">
-        <v>21</v>
+        <v>35</v>
       </c>
       <c r="U321">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="V321">
         <v>1</v>
@@ -28945,75 +28945,75 @@
         <v>0</v>
       </c>
       <c r="AB321">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AC321">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="322">
       <c r="A322">
-        <v>0</v>
+        <v>0.6</v>
       </c>
       <c r="B322">
-        <v>0</v>
+        <v>0.55</v>
       </c>
       <c r="C322">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="D322">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E322">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="F322">
         <v>5</v>
       </c>
       <c r="G322">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="H322">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="I322">
         <v>25</v>
       </c>
       <c r="J322">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="K322">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L322">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="M322">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="N322">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="O322">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="P322">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="Q322">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="R322">
         <v>8</v>
       </c>
       <c r="S322">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="T322">
         <v>35</v>
       </c>
       <c r="U322">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="V322">
         <v>1</v>
@@ -29034,75 +29034,75 @@
         <v>0</v>
       </c>
       <c r="AB322">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="AC322">
-        <v>3</v>
+        <v>10</v>
       </c>
     </row>
     <row r="323">
       <c r="A323">
-        <v>0.6</v>
+        <v>0</v>
       </c>
       <c r="B323">
-        <v>0.55</v>
+        <v>0.05</v>
       </c>
       <c r="C323">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="D323">
+        <v>12</v>
+      </c>
+      <c r="E323">
+        <v>5</v>
+      </c>
+      <c r="F323">
+        <v>17</v>
+      </c>
+      <c r="G323">
         <v>10</v>
       </c>
-      <c r="E323">
+      <c r="H323">
+        <v>30</v>
+      </c>
+      <c r="I323">
+        <v>23</v>
+      </c>
+      <c r="J323">
+        <v>4</v>
+      </c>
+      <c r="K323">
+        <v>20</v>
+      </c>
+      <c r="L323">
+        <v>18</v>
+      </c>
+      <c r="M323">
+        <v>9</v>
+      </c>
+      <c r="N323">
+        <v>6</v>
+      </c>
+      <c r="O323">
+        <v>22</v>
+      </c>
+      <c r="P323">
+        <v>19</v>
+      </c>
+      <c r="Q323">
+        <v>6</v>
+      </c>
+      <c r="R323">
+        <v>5</v>
+      </c>
+      <c r="S323">
         <v>10</v>
       </c>
-      <c r="F323">
-        <v>5</v>
-      </c>
-      <c r="G323">
-        <v>29</v>
-      </c>
-      <c r="H323">
-        <v>44</v>
-      </c>
-      <c r="I323">
-        <v>25</v>
-      </c>
-      <c r="J323">
-        <v>8</v>
-      </c>
-      <c r="K323">
-        <v>16</v>
-      </c>
-      <c r="L323">
-        <v>29</v>
-      </c>
-      <c r="M323">
-        <v>21</v>
-      </c>
-      <c r="N323">
-        <v>10</v>
-      </c>
-      <c r="O323">
-        <v>23</v>
-      </c>
-      <c r="P323">
-        <v>12</v>
-      </c>
-      <c r="Q323">
-        <v>8</v>
-      </c>
-      <c r="R323">
-        <v>8</v>
-      </c>
-      <c r="S323">
-        <v>14</v>
-      </c>
       <c r="T323">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="U323">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="V323">
         <v>1</v>
@@ -29123,78 +29123,78 @@
         <v>0</v>
       </c>
       <c r="AB323">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC323">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="324">
       <c r="A324">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="B324">
-        <v>0.05</v>
+        <v>0.3</v>
       </c>
       <c r="C324">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="D324">
+        <v>3</v>
+      </c>
+      <c r="E324">
+        <v>11</v>
+      </c>
+      <c r="F324">
+        <v>8</v>
+      </c>
+      <c r="G324">
+        <v>7</v>
+      </c>
+      <c r="H324">
+        <v>25</v>
+      </c>
+      <c r="I324">
+        <v>25</v>
+      </c>
+      <c r="J324">
+        <v>4</v>
+      </c>
+      <c r="K324">
+        <v>9</v>
+      </c>
+      <c r="L324">
+        <v>8</v>
+      </c>
+      <c r="M324">
+        <v>10</v>
+      </c>
+      <c r="N324">
+        <v>5</v>
+      </c>
+      <c r="O324">
+        <v>9</v>
+      </c>
+      <c r="P324">
+        <v>24</v>
+      </c>
+      <c r="Q324">
         <v>12</v>
       </c>
-      <c r="E324">
-        <v>5</v>
-      </c>
-      <c r="F324">
-        <v>17</v>
-      </c>
-      <c r="G324">
-        <v>10</v>
-      </c>
-      <c r="H324">
-        <v>30</v>
-      </c>
-      <c r="I324">
-        <v>23</v>
-      </c>
-      <c r="J324">
-        <v>4</v>
-      </c>
-      <c r="K324">
-        <v>20</v>
-      </c>
-      <c r="L324">
-        <v>18</v>
-      </c>
-      <c r="M324">
-        <v>9</v>
-      </c>
-      <c r="N324">
-        <v>6</v>
-      </c>
-      <c r="O324">
-        <v>22</v>
-      </c>
-      <c r="P324">
-        <v>19</v>
-      </c>
-      <c r="Q324">
-        <v>6</v>
-      </c>
       <c r="R324">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="S324">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="T324">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="U324">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V324">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W324">
         <v>0</v>
@@ -29215,96 +29215,96 @@
         <v>0</v>
       </c>
       <c r="AC324">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="325">
       <c r="A325">
-        <v>0.3</v>
+        <v>0.1</v>
       </c>
       <c r="B325">
-        <v>0.3</v>
+        <v>0.1</v>
       </c>
       <c r="C325">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D325">
         <v>3</v>
       </c>
       <c r="E325">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="F325">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G325">
-        <v>7</v>
+        <v>26</v>
       </c>
       <c r="H325">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="I325">
         <v>25</v>
       </c>
       <c r="J325">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="K325">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="L325">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="M325">
+        <v>6</v>
+      </c>
+      <c r="N325">
+        <v>7</v>
+      </c>
+      <c r="O325">
+        <v>11</v>
+      </c>
+      <c r="P325">
+        <v>7</v>
+      </c>
+      <c r="Q325">
+        <v>6</v>
+      </c>
+      <c r="R325">
+        <v>8</v>
+      </c>
+      <c r="S325">
+        <v>7</v>
+      </c>
+      <c r="T325">
+        <v>36</v>
+      </c>
+      <c r="U325">
+        <v>5</v>
+      </c>
+      <c r="V325">
+        <v>1</v>
+      </c>
+      <c r="W325">
+        <v>0</v>
+      </c>
+      <c r="X325">
+        <v>0</v>
+      </c>
+      <c r="Y325">
+        <v>0</v>
+      </c>
+      <c r="Z325">
+        <v>0</v>
+      </c>
+      <c r="AA325">
+        <v>0</v>
+      </c>
+      <c r="AB325">
+        <v>0</v>
+      </c>
+      <c r="AC325">
         <v>10</v>
-      </c>
-      <c r="N325">
-        <v>5</v>
-      </c>
-      <c r="O325">
-        <v>9</v>
-      </c>
-      <c r="P325">
-        <v>24</v>
-      </c>
-      <c r="Q325">
-        <v>12</v>
-      </c>
-      <c r="R325">
-        <v>8</v>
-      </c>
-      <c r="S325">
-        <v>11</v>
-      </c>
-      <c r="T325">
-        <v>37</v>
-      </c>
-      <c r="U325">
-        <v>0</v>
-      </c>
-      <c r="V325">
-        <v>0</v>
-      </c>
-      <c r="W325">
-        <v>0</v>
-      </c>
-      <c r="X325">
-        <v>0</v>
-      </c>
-      <c r="Y325">
-        <v>0</v>
-      </c>
-      <c r="Z325">
-        <v>0</v>
-      </c>
-      <c r="AA325">
-        <v>0</v>
-      </c>
-      <c r="AB325">
-        <v>0</v>
-      </c>
-      <c r="AC325">
-        <v>0</v>
       </c>
     </row>
     <row r="326">
@@ -29312,58 +29312,58 @@
         <v>0.1</v>
       </c>
       <c r="B326">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="C326">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D326">
         <v>3</v>
       </c>
       <c r="E326">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F326">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="G326">
-        <v>26</v>
+        <v>7</v>
       </c>
       <c r="H326">
-        <v>15</v>
+        <v>29</v>
       </c>
       <c r="I326">
         <v>25</v>
       </c>
       <c r="J326">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="K326">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="L326">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="M326">
         <v>6</v>
       </c>
       <c r="N326">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="O326">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="P326">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="Q326">
         <v>6</v>
       </c>
       <c r="R326">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="S326">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="T326">
         <v>36</v>
@@ -29372,7 +29372,7 @@
         <v>5</v>
       </c>
       <c r="V326">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W326">
         <v>0</v>
@@ -29393,72 +29393,72 @@
         <v>0</v>
       </c>
       <c r="AC326">
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="327">
       <c r="A327">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="B327">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="C327">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="D327">
         <v>3</v>
       </c>
       <c r="E327">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="F327">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="G327">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="H327">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="I327">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="J327">
         <v>5</v>
       </c>
       <c r="K327">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="L327">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="M327">
         <v>6</v>
       </c>
       <c r="N327">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="O327">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="P327">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="Q327">
         <v>6</v>
       </c>
       <c r="R327">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="S327">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="T327">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="U327">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="V327">
         <v>0</v>
@@ -29482,75 +29482,75 @@
         <v>0</v>
       </c>
       <c r="AC327">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="328">
       <c r="A328">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="B328">
-        <v>0</v>
+        <v>0.15</v>
       </c>
       <c r="C328">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D328">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="E328">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="F328">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="G328">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="H328">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="I328">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="J328">
         <v>5</v>
       </c>
       <c r="K328">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="L328">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="M328">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="N328">
         <v>7</v>
       </c>
       <c r="O328">
+        <v>18</v>
+      </c>
+      <c r="P328">
+        <v>15</v>
+      </c>
+      <c r="Q328">
+        <v>7</v>
+      </c>
+      <c r="R328">
+        <v>7</v>
+      </c>
+      <c r="S328">
         <v>11</v>
       </c>
-      <c r="P328">
-        <v>7</v>
-      </c>
-      <c r="Q328">
-        <v>6</v>
-      </c>
-      <c r="R328">
-        <v>4</v>
-      </c>
-      <c r="S328">
-        <v>6</v>
-      </c>
       <c r="T328">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="U328">
         <v>1</v>
       </c>
       <c r="V328">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W328">
         <v>0</v>
@@ -29571,185 +29571,185 @@
         <v>0</v>
       </c>
       <c r="AC328">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="329">
       <c r="A329">
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
       <c r="B329">
-        <v>0.15</v>
+        <v>0.3</v>
       </c>
       <c r="C329">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D329">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="E329">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="F329">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="G329">
         <v>7</v>
       </c>
       <c r="H329">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="I329">
+        <v>23</v>
+      </c>
+      <c r="J329">
+        <v>11</v>
+      </c>
+      <c r="K329">
+        <v>14</v>
+      </c>
+      <c r="L329">
         <v>24</v>
       </c>
-      <c r="J329">
-        <v>5</v>
-      </c>
-      <c r="K329">
+      <c r="M329">
+        <v>16</v>
+      </c>
+      <c r="N329">
+        <v>17</v>
+      </c>
+      <c r="O329">
+        <v>19</v>
+      </c>
+      <c r="P329">
+        <v>10</v>
+      </c>
+      <c r="Q329">
+        <v>12</v>
+      </c>
+      <c r="R329">
+        <v>14</v>
+      </c>
+      <c r="S329">
         <v>15</v>
       </c>
-      <c r="L329">
-        <v>16</v>
-      </c>
-      <c r="M329">
-        <v>8</v>
-      </c>
-      <c r="N329">
-        <v>7</v>
-      </c>
-      <c r="O329">
-        <v>18</v>
-      </c>
-      <c r="P329">
-        <v>15</v>
-      </c>
-      <c r="Q329">
-        <v>7</v>
-      </c>
-      <c r="R329">
-        <v>7</v>
-      </c>
-      <c r="S329">
-        <v>11</v>
-      </c>
       <c r="T329">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="U329">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="V329">
         <v>1</v>
       </c>
       <c r="W329">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X329">
         <v>0</v>
       </c>
       <c r="Y329">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z329">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA329">
         <v>0</v>
       </c>
       <c r="AB329">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC329">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="330">
       <c r="A330">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="B330">
-        <v>0.3</v>
+        <v>0</v>
       </c>
       <c r="C330">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="D330">
         <v>3</v>
       </c>
       <c r="E330">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="F330">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="G330">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="H330">
-        <v>35</v>
+        <v>19</v>
       </c>
       <c r="I330">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="J330">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="K330">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="L330">
-        <v>24</v>
+        <v>6</v>
       </c>
       <c r="M330">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="N330">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="O330">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="P330">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="Q330">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="R330">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="S330">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="T330">
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="U330">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="V330">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W330">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X330">
         <v>0</v>
       </c>
       <c r="Y330">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z330">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA330">
         <v>0</v>
       </c>
       <c r="AB330">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC330">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="331">
@@ -29760,22 +29760,22 @@
         <v>0</v>
       </c>
       <c r="C331">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D331">
         <v>3</v>
       </c>
       <c r="E331">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F331">
         <v>5</v>
       </c>
       <c r="G331">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H331">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="I331">
         <v>24</v>
@@ -29784,13 +29784,13 @@
         <v>4</v>
       </c>
       <c r="K331">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="L331">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="M331">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="N331">
         <v>7</v>
@@ -29799,25 +29799,25 @@
         <v>8</v>
       </c>
       <c r="P331">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="Q331">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="R331">
         <v>5</v>
       </c>
       <c r="S331">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="T331">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="U331">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V331">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W331">
         <v>0</v>
@@ -29835,10 +29835,10 @@
         <v>0</v>
       </c>
       <c r="AB331">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC331">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="332">
@@ -29861,10 +29861,10 @@
         <v>5</v>
       </c>
       <c r="G332">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H332">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="I332">
         <v>24</v>
@@ -29873,34 +29873,34 @@
         <v>4</v>
       </c>
       <c r="K332">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="L332">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="M332">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="N332">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="O332">
         <v>8</v>
       </c>
       <c r="P332">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="Q332">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="R332">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="S332">
         <v>4</v>
       </c>
       <c r="T332">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="U332">
         <v>1</v>
@@ -29924,75 +29924,75 @@
         <v>0</v>
       </c>
       <c r="AB332">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC332">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="333">
       <c r="A333">
-        <v>0</v>
+        <v>0.35</v>
       </c>
       <c r="B333">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="C333">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="D333">
         <v>3</v>
       </c>
       <c r="E333">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F333">
         <v>5</v>
       </c>
       <c r="G333">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H333">
+        <v>30</v>
+      </c>
+      <c r="I333">
+        <v>25</v>
+      </c>
+      <c r="J333">
+        <v>9</v>
+      </c>
+      <c r="K333">
+        <v>15</v>
+      </c>
+      <c r="L333">
+        <v>16</v>
+      </c>
+      <c r="M333">
+        <v>8</v>
+      </c>
+      <c r="N333">
+        <v>8</v>
+      </c>
+      <c r="O333">
         <v>10</v>
       </c>
-      <c r="I333">
-        <v>24</v>
-      </c>
-      <c r="J333">
-        <v>4</v>
-      </c>
-      <c r="K333">
-        <v>8</v>
-      </c>
-      <c r="L333">
-        <v>6</v>
-      </c>
-      <c r="M333">
-        <v>9</v>
-      </c>
-      <c r="N333">
-        <v>9</v>
-      </c>
-      <c r="O333">
-        <v>8</v>
-      </c>
       <c r="P333">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="Q333">
         <v>7</v>
       </c>
       <c r="R333">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="S333">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="T333">
-        <v>13</v>
+        <v>32</v>
       </c>
       <c r="U333">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="V333">
         <v>1</v>
@@ -30016,72 +30016,72 @@
         <v>0</v>
       </c>
       <c r="AC333">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="334">
       <c r="A334">
-        <v>0.35</v>
+        <v>0.15</v>
       </c>
       <c r="B334">
         <v>0.2</v>
       </c>
       <c r="C334">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="D334">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E334">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F334">
         <v>5</v>
       </c>
       <c r="G334">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H334">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="I334">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="J334">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="K334">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="L334">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="M334">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="N334">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="O334">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="P334">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="Q334">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="R334">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="S334">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="T334">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="U334">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="V334">
         <v>1</v>
@@ -30093,7 +30093,7 @@
         <v>0</v>
       </c>
       <c r="Y334">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="Z334">
         <v>0</v>
@@ -30105,7 +30105,7 @@
         <v>0</v>
       </c>
       <c r="AC334">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="335">
@@ -30377,73 +30377,73 @@
     </row>
     <row r="338">
       <c r="A338">
-        <v>0</v>
+        <v>0.15</v>
       </c>
       <c r="B338">
-        <v>0</v>
+        <v>0.15</v>
       </c>
       <c r="C338">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D338">
         <v>3</v>
       </c>
       <c r="E338">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="F338">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G338">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="H338">
+        <v>25</v>
+      </c>
+      <c r="I338">
+        <v>18</v>
+      </c>
+      <c r="J338">
+        <v>7</v>
+      </c>
+      <c r="K338">
+        <v>12</v>
+      </c>
+      <c r="L338">
+        <v>10</v>
+      </c>
+      <c r="M338">
+        <v>14</v>
+      </c>
+      <c r="N338">
+        <v>19</v>
+      </c>
+      <c r="O338">
+        <v>10</v>
+      </c>
+      <c r="P338">
+        <v>13</v>
+      </c>
+      <c r="Q338">
+        <v>6</v>
+      </c>
+      <c r="R338">
+        <v>6</v>
+      </c>
+      <c r="S338">
+        <v>8</v>
+      </c>
+      <c r="T338">
         <v>16</v>
       </c>
-      <c r="I338">
-        <v>25</v>
-      </c>
-      <c r="J338">
-        <v>4</v>
-      </c>
-      <c r="K338">
-        <v>11</v>
-      </c>
-      <c r="L338">
-        <v>8</v>
-      </c>
-      <c r="M338">
-        <v>5</v>
-      </c>
-      <c r="N338">
-        <v>6</v>
-      </c>
-      <c r="O338">
-        <v>8</v>
-      </c>
-      <c r="P338">
-        <v>7</v>
-      </c>
-      <c r="Q338">
-        <v>6</v>
-      </c>
-      <c r="R338">
-        <v>6</v>
-      </c>
-      <c r="S338">
-        <v>6</v>
-      </c>
-      <c r="T338">
-        <v>19</v>
-      </c>
       <c r="U338">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="V338">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W338">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X338">
         <v>0</v>
@@ -30461,7 +30461,7 @@
         <v>0</v>
       </c>
       <c r="AC338">
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="339">
@@ -30475,58 +30475,58 @@
         <v>6</v>
       </c>
       <c r="D339">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E339">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="F339">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="G339">
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="H339">
+        <v>18</v>
+      </c>
+      <c r="I339">
         <v>25</v>
       </c>
-      <c r="I339">
-        <v>18</v>
-      </c>
       <c r="J339">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="K339">
         <v>12</v>
       </c>
       <c r="L339">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="M339">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="N339">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="O339">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="P339">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="Q339">
         <v>6</v>
       </c>
       <c r="R339">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="S339">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="T339">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="U339">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="V339">
         <v>1</v>
@@ -30550,7 +30550,7 @@
         <v>0</v>
       </c>
       <c r="AC339">
-        <v>9</v>
+        <v>1</v>
       </c>
     </row>
     <row r="340">
@@ -30561,67 +30561,67 @@
         <v>0.15</v>
       </c>
       <c r="C340">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D340">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E340">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="F340">
         <v>9</v>
       </c>
       <c r="G340">
-        <v>27</v>
+        <v>9</v>
       </c>
       <c r="H340">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="I340">
         <v>25</v>
       </c>
       <c r="J340">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="K340">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="L340">
+        <v>17</v>
+      </c>
+      <c r="M340">
+        <v>10</v>
+      </c>
+      <c r="N340">
+        <v>10</v>
+      </c>
+      <c r="O340">
+        <v>9</v>
+      </c>
+      <c r="P340">
+        <v>17</v>
+      </c>
+      <c r="Q340">
+        <v>10</v>
+      </c>
+      <c r="R340">
+        <v>8</v>
+      </c>
+      <c r="S340">
         <v>11</v>
       </c>
-      <c r="M340">
-        <v>5</v>
-      </c>
-      <c r="N340">
-        <v>12</v>
-      </c>
-      <c r="O340">
-        <v>9</v>
-      </c>
-      <c r="P340">
-        <v>9</v>
-      </c>
-      <c r="Q340">
-        <v>6</v>
-      </c>
-      <c r="R340">
-        <v>9</v>
-      </c>
-      <c r="S340">
-        <v>5</v>
-      </c>
       <c r="T340">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="U340">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="V340">
         <v>1</v>
       </c>
       <c r="W340">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X340">
         <v>0</v>
@@ -30630,16 +30630,16 @@
         <v>0</v>
       </c>
       <c r="Z340">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA340">
         <v>0</v>
       </c>
       <c r="AB340">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AC340">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="341">
@@ -30650,67 +30650,67 @@
         <v>0.15</v>
       </c>
       <c r="C341">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D341">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E341">
+        <v>9</v>
+      </c>
+      <c r="F341">
+        <v>9</v>
+      </c>
+      <c r="G341">
+        <v>7</v>
+      </c>
+      <c r="H341">
+        <v>23</v>
+      </c>
+      <c r="I341">
+        <v>22</v>
+      </c>
+      <c r="J341">
+        <v>7</v>
+      </c>
+      <c r="K341">
+        <v>6</v>
+      </c>
+      <c r="L341">
+        <v>8</v>
+      </c>
+      <c r="M341">
+        <v>8</v>
+      </c>
+      <c r="N341">
+        <v>6</v>
+      </c>
+      <c r="O341">
         <v>11</v>
       </c>
-      <c r="F341">
-        <v>9</v>
-      </c>
-      <c r="G341">
-        <v>9</v>
-      </c>
-      <c r="H341">
-        <v>29</v>
-      </c>
-      <c r="I341">
-        <v>25</v>
-      </c>
-      <c r="J341">
-        <v>4</v>
-      </c>
-      <c r="K341">
-        <v>9</v>
-      </c>
-      <c r="L341">
-        <v>17</v>
-      </c>
-      <c r="M341">
-        <v>10</v>
-      </c>
-      <c r="N341">
-        <v>10</v>
-      </c>
-      <c r="O341">
-        <v>9</v>
-      </c>
       <c r="P341">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="Q341">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="R341">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="S341">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="T341">
         <v>32</v>
       </c>
       <c r="U341">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="V341">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W341">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X341">
         <v>0</v>
@@ -30719,81 +30719,81 @@
         <v>0</v>
       </c>
       <c r="Z341">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA341">
         <v>0</v>
       </c>
       <c r="AB341">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AC341">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="342">
       <c r="A342">
-        <v>0.15</v>
+        <v>0.35</v>
       </c>
       <c r="B342">
-        <v>0.15</v>
+        <v>0.25</v>
       </c>
       <c r="C342">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D342">
         <v>3</v>
       </c>
       <c r="E342">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="F342">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G342">
         <v>7</v>
       </c>
       <c r="H342">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="I342">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="J342">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="K342">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="L342">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="M342">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="N342">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="O342">
         <v>11</v>
       </c>
       <c r="P342">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="Q342">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="R342">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="S342">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="T342">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="U342">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="V342">
         <v>0</v>
@@ -30817,78 +30817,78 @@
         <v>0</v>
       </c>
       <c r="AC342">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="343">
       <c r="A343">
-        <v>0.35</v>
+        <v>0.1</v>
       </c>
       <c r="B343">
-        <v>0.25</v>
+        <v>0.15</v>
       </c>
       <c r="C343">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D343">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="E343">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="F343">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="G343">
         <v>7</v>
       </c>
       <c r="H343">
-        <v>33</v>
+        <v>18</v>
       </c>
       <c r="I343">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J343">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="K343">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="L343">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="M343">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="N343">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="O343">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="P343">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="Q343">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="R343">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="S343">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="T343">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="U343">
         <v>6</v>
       </c>
       <c r="V343">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="W343">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X343">
         <v>0</v>
@@ -30906,78 +30906,78 @@
         <v>0</v>
       </c>
       <c r="AC343">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="344">
       <c r="A344">
-        <v>0.1</v>
+        <v>0.4</v>
       </c>
       <c r="B344">
-        <v>0.15</v>
+        <v>0.8</v>
       </c>
       <c r="C344">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="D344">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="E344">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="F344">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="G344">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="H344">
-        <v>18</v>
+        <v>47</v>
       </c>
       <c r="I344">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="J344">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="K344">
-        <v>10</v>
+        <v>28</v>
       </c>
       <c r="L344">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="M344">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="N344">
+        <v>23</v>
+      </c>
+      <c r="O344">
+        <v>26</v>
+      </c>
+      <c r="P344">
         <v>13</v>
       </c>
-      <c r="O344">
-        <v>9</v>
-      </c>
-      <c r="P344">
-        <v>6</v>
-      </c>
       <c r="Q344">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="R344">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="S344">
-        <v>4</v>
+        <v>19</v>
       </c>
       <c r="T344">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="U344">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="V344">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="W344">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X344">
         <v>0</v>
@@ -30995,75 +30995,75 @@
         <v>0</v>
       </c>
       <c r="AC344">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="345">
       <c r="A345">
-        <v>0.4</v>
+        <v>0.15</v>
       </c>
       <c r="B345">
-        <v>0.8</v>
+        <v>0.15</v>
       </c>
       <c r="C345">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="D345">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E345">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="F345">
+        <v>8</v>
+      </c>
+      <c r="G345">
+        <v>7</v>
+      </c>
+      <c r="H345">
+        <v>23</v>
+      </c>
+      <c r="I345">
+        <v>25</v>
+      </c>
+      <c r="J345">
+        <v>5</v>
+      </c>
+      <c r="K345">
+        <v>11</v>
+      </c>
+      <c r="L345">
         <v>12</v>
       </c>
-      <c r="G345">
-        <v>11</v>
-      </c>
-      <c r="H345">
-        <v>47</v>
-      </c>
-      <c r="I345">
-        <v>19</v>
-      </c>
-      <c r="J345">
-        <v>17</v>
-      </c>
-      <c r="K345">
-        <v>28</v>
-      </c>
-      <c r="L345">
-        <v>19</v>
-      </c>
       <c r="M345">
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="N345">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="O345">
-        <v>26</v>
+        <v>8</v>
       </c>
       <c r="P345">
         <v>13</v>
       </c>
       <c r="Q345">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="R345">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="S345">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="T345">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="U345">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="V345">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W345">
         <v>0</v>
@@ -31089,28 +31089,28 @@
     </row>
     <row r="346">
       <c r="A346">
-        <v>0.15</v>
+        <v>0.1</v>
       </c>
       <c r="B346">
-        <v>0.15</v>
+        <v>0.1</v>
       </c>
       <c r="C346">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D346">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E346">
         <v>6</v>
       </c>
       <c r="F346">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G346">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H346">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="I346">
         <v>25</v>
@@ -31119,40 +31119,40 @@
         <v>5</v>
       </c>
       <c r="K346">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="L346">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="M346">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="N346">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="O346">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="P346">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="Q346">
         <v>6</v>
       </c>
       <c r="R346">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="S346">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="T346">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="U346">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="V346">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W346">
         <v>0</v>
@@ -31173,95 +31173,6 @@
         <v>0</v>
       </c>
       <c r="AC346">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="347">
-      <c r="A347">
-        <v>0.1</v>
-      </c>
-      <c r="B347">
-        <v>0.1</v>
-      </c>
-      <c r="C347">
-        <v>5</v>
-      </c>
-      <c r="D347">
-        <v>3</v>
-      </c>
-      <c r="E347">
-        <v>6</v>
-      </c>
-      <c r="F347">
-        <v>7</v>
-      </c>
-      <c r="G347">
-        <v>8</v>
-      </c>
-      <c r="H347">
-        <v>28</v>
-      </c>
-      <c r="I347">
-        <v>25</v>
-      </c>
-      <c r="J347">
-        <v>5</v>
-      </c>
-      <c r="K347">
-        <v>6</v>
-      </c>
-      <c r="L347">
-        <v>20</v>
-      </c>
-      <c r="M347">
-        <v>13</v>
-      </c>
-      <c r="N347">
-        <v>6</v>
-      </c>
-      <c r="O347">
-        <v>13</v>
-      </c>
-      <c r="P347">
-        <v>8</v>
-      </c>
-      <c r="Q347">
-        <v>6</v>
-      </c>
-      <c r="R347">
-        <v>5</v>
-      </c>
-      <c r="S347">
-        <v>5</v>
-      </c>
-      <c r="T347">
-        <v>33</v>
-      </c>
-      <c r="U347">
-        <v>1</v>
-      </c>
-      <c r="V347">
-        <v>1</v>
-      </c>
-      <c r="W347">
-        <v>0</v>
-      </c>
-      <c r="X347">
-        <v>0</v>
-      </c>
-      <c r="Y347">
-        <v>0</v>
-      </c>
-      <c r="Z347">
-        <v>0</v>
-      </c>
-      <c r="AA347">
-        <v>0</v>
-      </c>
-      <c r="AB347">
-        <v>0</v>
-      </c>
-      <c r="AC347">
         <v>1</v>
       </c>
     </row>

</xml_diff>